<commit_message>
Add user guide and implement sound effects for spinning wheel
</commit_message>
<xml_diff>
--- a/LuckySpin/LuckySpin/bin/Lucky Wheel/Config/INPUT.xlsx
+++ b/LuckySpin/LuckySpin/bin/Lucky Wheel/Config/INPUT.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="e:\Lucky Spin\Lucky Spin\LuckySpin\LuckySpin\bin\Lucky Wheel\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Lucky Spin\Lucky Spin\LuckySpin\LuckySpin\bin\Lucky Wheel\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6173B86-2CDF-4E6A-96F9-39AFBF511EDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3480FD-BBFE-4FD8-9C42-3585E8E710A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="18000" windowHeight="9270" xr2:uid="{ACD92B7C-6A47-4C25-BFEA-2140BAC1F5F0}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="15">
   <si>
     <t>NAME</t>
   </si>
@@ -37,40 +37,34 @@
     <t>IMAGE</t>
   </si>
   <si>
-    <t>1.000.000 VNÄ</t>
-  </si>
-  <si>
     <t>money2.png</t>
   </si>
   <si>
-    <t>500.000 VNÄ</t>
-  </si>
-  <si>
-    <t>money1.png</t>
-  </si>
-  <si>
-    <t>100.000 VNÄ</t>
-  </si>
-  <si>
-    <t>gift1.png</t>
-  </si>
-  <si>
-    <t>50.000 VNÄ</t>
-  </si>
-  <si>
-    <t>ChÃºc may máº¯n láº§n sau</t>
-  </si>
-  <si>
     <t>sad.png</t>
   </si>
   <si>
-    <t>20.000 VNÄ</t>
-  </si>
-  <si>
-    <t>10.000 VNÄ</t>
-  </si>
-  <si>
-    <t>5.000 VNÄ</t>
+    <t>1tr</t>
+  </si>
+  <si>
+    <t>500k</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>50k</t>
+  </si>
+  <si>
+    <t>chúc bạn may mắn lần sau</t>
+  </si>
+  <si>
+    <t>20k</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>5k</t>
   </si>
 </sst>
 </file>
@@ -933,9 +927,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{559176F0-C073-4C8E-8C83-9D31F9E7064C}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -956,7 +956,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -965,84 +965,90 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
       <c r="D4" t="b">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7" t="b">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D8" t="b">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D9" t="b">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>